<commit_message>
Remove unnecessary test files and deployment artifacts
</commit_message>
<xml_diff>
--- a/backend/workout_app_data.xlsx
+++ b/backend/workout_app_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivansakthivel/Documents/Hash_Github/workout/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B917A-2841-824D-B25E-24E28A5E6A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1CACAF-2569-FE42-A910-0227FD54C115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15020" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>user_id</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>created_at</t>
+  </si>
+  <si>
+    <t>Sivan</t>
+  </si>
+  <si>
+    <t>5555</t>
+  </si>
+  <si>
+    <t>2026-01-12T20:00:11.279442</t>
   </si>
   <si>
     <t>date</t>
@@ -95,11 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,11 +412,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -422,6 +430,20 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -431,24 +453,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>46023</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>46024</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>46025</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>46026</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>46027</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>46028</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>46029</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>46030</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>46031</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>46032</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>46033</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>46034</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>